<commit_message>
added additional test cases for com.bmwusa
</commit_message>
<xml_diff>
--- a/com.bmwusa/src/test/resources/testData/bmwRegisterTestData.xlsx
+++ b/com.bmwusa/src/test/resources/testData/bmwRegisterTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="14295" windowHeight="5910" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="14295" windowHeight="5910" tabRatio="814" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="register" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,16 @@
     <sheet name="invalid_password" sheetId="3" r:id="rId3"/>
     <sheet name="different_password" sheetId="4" r:id="rId4"/>
     <sheet name="valid_credentials" sheetId="5" r:id="rId5"/>
+    <sheet name="used_password" sheetId="6" r:id="rId6"/>
+    <sheet name="valid_login" sheetId="7" r:id="rId7"/>
+    <sheet name="invalid_login" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="32">
   <si>
     <t>first_name</t>
   </si>
@@ -102,6 +105,18 @@
   </si>
   <si>
     <t>yanira1243211@gmail.com</t>
+  </si>
+  <si>
+    <t>bmw@gmail.com</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>12345678a</t>
+  </si>
+  <si>
+    <t>erj.juridico@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -624,7 +639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -805,7 +820,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -858,4 +873,139 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="yanira124325@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2">
+        <v>12345678</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>